<commit_message>
command m, q or y, for month, quarter or year form
</commit_message>
<xml_diff>
--- a/public/Spreadsheets/customerOverview.xlsx
+++ b/public/Spreadsheets/customerOverview.xlsx
@@ -29,40 +29,40 @@
     <t>Bought Kwh --&gt;</t>
   </si>
   <si>
-    <t>06-2022</t>
-  </si>
-  <si>
-    <t>07-2022</t>
-  </si>
-  <si>
-    <t>08-2022</t>
-  </si>
-  <si>
-    <t>09-2022</t>
-  </si>
-  <si>
-    <t>10-2022</t>
-  </si>
-  <si>
-    <t>11-2022</t>
-  </si>
-  <si>
-    <t>12-2022</t>
-  </si>
-  <si>
-    <t>01-2023</t>
-  </si>
-  <si>
-    <t>02-2023</t>
-  </si>
-  <si>
-    <t>03-2023</t>
-  </si>
-  <si>
-    <t>04-2023</t>
-  </si>
-  <si>
-    <t>05-2023</t>
+    <t>06-2022 - 07-2022</t>
+  </si>
+  <si>
+    <t>07-2022 - 08-2022</t>
+  </si>
+  <si>
+    <t>08-2022 - 09-2022</t>
+  </si>
+  <si>
+    <t>09-2022 - 10-2022</t>
+  </si>
+  <si>
+    <t>10-2022 - 11-2022</t>
+  </si>
+  <si>
+    <t>11-2022 - 12-2022</t>
+  </si>
+  <si>
+    <t>12-2022 - 01-2023</t>
+  </si>
+  <si>
+    <t>01-2023 - 02-2023</t>
+  </si>
+  <si>
+    <t>02-2023 - 03-2023</t>
+  </si>
+  <si>
+    <t>03-2023 - 04-2023</t>
+  </si>
+  <si>
+    <t>04-2023 - 05-2023</t>
+  </si>
+  <si>
+    <t>05-2023 - 06-2023</t>
   </si>
   <si>
     <t>mick de muis</t>
@@ -730,18 +730,18 @@
     <col min="2" max="2" width="19.995" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="21.138" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">

</xml_diff>

<commit_message>
overview of revenue per month
</commit_message>
<xml_diff>
--- a/public/Spreadsheets/customerOverview.xlsx
+++ b/public/Spreadsheets/customerOverview.xlsx
@@ -146,7 +146,7 @@
     <t>bas man</t>
   </si>
   <si>
-    <t>€ 1981.22</t>
+    <t>€ 1700.19</t>
   </si>
   <si>
     <t>49.8 Kwh</t>
@@ -188,7 +188,7 @@
     <t>Papageno Smithe</t>
   </si>
   <si>
-    <t>€ 1192</t>
+    <t>€ 1649.48</t>
   </si>
   <si>
     <t>98.93 Kwh</t>
@@ -227,7 +227,7 @@
     <t>Aldwin Cheavin</t>
   </si>
   <si>
-    <t>€ 1336.98</t>
+    <t>€ 1342.54</t>
   </si>
   <si>
     <t>46.38 Kwh</t>
@@ -266,7 +266,7 @@
     <t>Amerigo Bridat</t>
   </si>
   <si>
-    <t>€ 1413.27</t>
+    <t>€ 1460.25</t>
   </si>
   <si>
     <t>66.32 Kwh</t>
@@ -302,7 +302,7 @@
     <t>Melissa Ciciotti</t>
   </si>
   <si>
-    <t>€ 2186.98</t>
+    <t>€ 1448.54</t>
   </si>
   <si>
     <t>80.83 Kwh</t>
@@ -338,7 +338,7 @@
     <t>Torrey Rawlison</t>
   </si>
   <si>
-    <t>€ 1524.3</t>
+    <t>€ 1423.82</t>
   </si>
   <si>
     <t>155.53 Kwh</t>
@@ -816,22 +816,22 @@
       <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -948,28 +948,28 @@
       <c r="G5" t="s">
         <v>60</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>61</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>62</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>63</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>64</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>65</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>66</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>67</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -992,28 +992,28 @@
       <c r="G6" t="s">
         <v>73</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>74</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>75</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>76</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>77</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>78</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>79</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>80</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1027,34 +1027,34 @@
       <c r="C7" t="s">
         <v>83</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>84</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>85</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>86</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>87</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>88</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>89</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>90</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>91</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>92</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1074,28 +1074,28 @@
       <c r="F8" t="s">
         <v>97</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>98</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>99</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>100</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>101</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>102</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>103</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
         <v>104</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1118,25 +1118,25 @@
       <c r="G9" t="s">
         <v>110</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>111</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>112</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>113</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>114</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>115</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>116</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>